<commit_message>
Accept time-series BAU data for soft costs of onshore wind, offshore wind, solar PV, and distributed solar PV.  Use $/MW instead of percentage units. (#78)
</commit_message>
<xml_diff>
--- a/InputData/bldgs/CpUDSC/Cost per Unit Dist Solar Cap.xlsx
+++ b/InputData/bldgs/CpUDSC/Cost per Unit Dist Solar Cap.xlsx
@@ -1,28 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us\InputData\bldgs\CpUDSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\bldgs\CpUDSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F11FE36-41F2-4CC9-B172-CB91A4E38E2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="19425" windowHeight="11025"/>
+    <workbookView xWindow="3135" yWindow="1260" windowWidth="21600" windowHeight="14550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="DC to AC" sheetId="5" r:id="rId2"/>
     <sheet name="NREL ATB" sheetId="7" r:id="rId3"/>
-    <sheet name="CpUDSC" sheetId="2" r:id="rId4"/>
+    <sheet name="Soft Cost Data" sheetId="9" r:id="rId4"/>
+    <sheet name="CpUDSC-totalcost" sheetId="2" r:id="rId5"/>
+    <sheet name="CpUDSC-softcosts" sheetId="8" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
   <si>
     <t>CpUDSC Cost per Unit Distributed Solar Capacity</t>
   </si>
@@ -30,9 +43,6 @@
     <t>Sources:</t>
   </si>
   <si>
-    <t>Distributed Solar Cap Cost ($/MW)</t>
-  </si>
-  <si>
     <t>Solar DC to AC Derate Value</t>
   </si>
   <si>
@@ -139,16 +149,73 @@
   </si>
   <si>
     <t>We use the ATB "Moderate" case</t>
+  </si>
+  <si>
+    <t>Solar PV</t>
+  </si>
+  <si>
+    <t>Solar PV Type</t>
+  </si>
+  <si>
+    <t>Non-Hardware Cost %</t>
+  </si>
+  <si>
+    <t>Residential</t>
+  </si>
+  <si>
+    <t>Commercial</t>
+  </si>
+  <si>
+    <t>Utility-Scale</t>
+  </si>
+  <si>
+    <t>Share of Costs that are Soft Costs</t>
+  </si>
+  <si>
+    <t>U.S. Solar Photovoltaic System Cost Benchmark: Q1 2018</t>
+  </si>
+  <si>
+    <t>https://www.nrel.gov/docs/fy17osti/68925.pdf</t>
+  </si>
+  <si>
+    <t>Page viii, Figure ES-2</t>
+  </si>
+  <si>
+    <t>"Soft costs" (non-hardware costs, such as the cost of installation)</t>
+  </si>
+  <si>
+    <t>are a subset of the total costs.  Soft costs are not subject to</t>
+  </si>
+  <si>
+    <t>reductions from endogenous learning.</t>
+  </si>
+  <si>
+    <t>For distributed PV on buildings, we use the average</t>
+  </si>
+  <si>
+    <t>of residential and commercial soft cost shares.</t>
+  </si>
+  <si>
+    <t>Buildings</t>
+  </si>
+  <si>
+    <t>Unit: $/MW</t>
+  </si>
+  <si>
+    <t>Distributed Solar Soft Costs</t>
+  </si>
+  <si>
+    <t>Distributed Solar Total Cap Cost</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,8 +276,16 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -220,6 +295,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -389,7 +476,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -422,21 +509,29 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="12"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="13">
-    <cellStyle name="Body: normal cell" xfId="1"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="2"/>
-    <cellStyle name="Footnotes: all except top row" xfId="3"/>
-    <cellStyle name="Footnotes: top row" xfId="4"/>
-    <cellStyle name="Header: bottom row" xfId="5"/>
-    <cellStyle name="Header: top rows" xfId="6"/>
+    <cellStyle name="Body: normal cell" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Footnotes: all except top row" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Footnotes: top row" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Header: bottom row" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Header: top rows" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Hyperlink" xfId="12" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="7"/>
+    <cellStyle name="Hyperlink 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Parent row" xfId="8"/>
-    <cellStyle name="Section Break" xfId="9"/>
-    <cellStyle name="Section Break: parent row" xfId="10"/>
-    <cellStyle name="Table title" xfId="11"/>
+    <cellStyle name="Parent row" xfId="8" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Section Break" xfId="9" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Section Break: parent row" xfId="10" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Table title" xfId="11" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -527,6 +622,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -562,6 +674,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -737,141 +866,185 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="50.1328125" customWidth="1"/>
+    <col min="2" max="2" width="50.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>2020</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>2015</v>
       </c>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A17" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>38</v>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B21" r:id="rId1" xr:uid="{1CA9C921-186B-4B9E-A32E-9A5AEB5517FB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.85899999999999999</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
     </row>
   </sheetData>
@@ -881,25 +1054,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AI23"/>
   <sheetViews>
-    <sheetView topLeftCell="R3" workbookViewId="0">
-      <selection activeCell="R10" sqref="A10:XFD10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.796875" customWidth="1"/>
-    <col min="2" max="2" width="33.265625" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.45">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="C3">
         <v>2018</v>
       </c>
@@ -1000,12 +1171,12 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4">
         <v>3054.318209074861</v>
@@ -1107,9 +1278,9 @@
         <v>602.42092125560248</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5">
         <v>3054.318209074861</v>
@@ -1211,9 +1382,9 @@
         <v>857.6570833640435</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6">
         <v>3054.318209074861</v>
@@ -1315,9 +1486,9 @@
         <v>1124.6145820191289</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7">
         <v>3054.318209074861</v>
@@ -1419,9 +1590,9 @@
         <v>602.42092125560248</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8">
         <v>3054.318209074861</v>
@@ -1523,9 +1694,9 @@
         <v>857.6570833640435</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9">
         <v>3054.318209074861</v>
@@ -1627,9 +1798,9 @@
         <v>1124.6145820191289</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10">
         <v>3054.318209074861</v>
@@ -1731,9 +1902,9 @@
         <v>602.42092125560248</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11">
         <v>3054.318209074861</v>
@@ -1835,9 +2006,9 @@
         <v>857.6570833640435</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12">
         <v>3054.318209074861</v>
@@ -1939,9 +2110,9 @@
         <v>1124.6145820191289</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13">
         <v>3054.318209074861</v>
@@ -2043,9 +2214,9 @@
         <v>602.42092125560248</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14">
         <v>3054.318209074861</v>
@@ -2147,9 +2318,9 @@
         <v>857.6570833640435</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15">
         <v>3054.318209074861</v>
@@ -2251,9 +2422,9 @@
         <v>1124.6145820191289</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16">
         <v>3054.318209074861</v>
@@ -2355,9 +2526,9 @@
         <v>602.42092125560248</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17">
         <v>3054.318209074861</v>
@@ -2459,9 +2630,9 @@
         <v>857.6570833640435</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18">
         <v>3054.318209074861</v>
@@ -2563,9 +2734,9 @@
         <v>1124.6145820191289</v>
       </c>
     </row>
-    <row r="20" spans="1:35" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -2573,9 +2744,9 @@
       <c r="E20" s="9"/>
       <c r="F20" s="10"/>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
@@ -2583,9 +2754,9 @@
       <c r="E21" s="12"/>
       <c r="F21" s="13"/>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
@@ -2593,9 +2764,9 @@
       <c r="E22" s="12"/>
       <c r="F22" s="13"/>
     </row>
-    <row r="23" spans="1:35" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -2615,312 +2786,705 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF31DC84-8E1C-4B41-A58F-99DEB8033653}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="16">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="16">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="16">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="17">
+        <f>AVERAGE(B4:B5)</f>
+        <v>0.59499999999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet3">
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B33"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.1328125" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>54</v>
+      </c>
       <c r="B1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2019</v>
       </c>
       <c r="B2" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH(CpUDSC!A2,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A2,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
         <v>3255232.9117624536</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2020</v>
       </c>
       <c r="B3" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH(CpUDSC!A3,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A3,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
         <v>3078322.0757814161</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2021</v>
       </c>
       <c r="B4" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH(CpUDSC!A4,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A4,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
         <v>2901411.2398003791</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2022</v>
       </c>
       <c r="B5" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH(CpUDSC!A5,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A5,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
         <v>2724500.4038193417</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2023</v>
       </c>
       <c r="B6" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH(CpUDSC!A6,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A6,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
         <v>2547589.5678383047</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2024</v>
       </c>
       <c r="B7" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH(CpUDSC!A7,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A7,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
         <v>2370678.7318572667</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2025</v>
       </c>
       <c r="B8" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH(CpUDSC!A8,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A8,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
         <v>2193767.8958762302</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2026</v>
       </c>
       <c r="B9" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH(CpUDSC!A9,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A9,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
         <v>2016857.059895193</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2027</v>
       </c>
       <c r="B10" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH(CpUDSC!A10,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A10,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
         <v>1839946.223914156</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2028</v>
       </c>
       <c r="B11" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH(CpUDSC!A11,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A11,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
         <v>1663035.387933119</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2029</v>
       </c>
       <c r="B12" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH(CpUDSC!A12,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A12,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
         <v>1486124.551952082</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2030</v>
       </c>
       <c r="B13" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH(CpUDSC!A13,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A13,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
         <v>1309213.7159710464</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2031</v>
       </c>
       <c r="B14" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH(CpUDSC!A14,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A14,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
         <v>1293674.8627315189</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2032</v>
       </c>
       <c r="B15" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH(CpUDSC!A15,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A15,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
         <v>1278136.009491991</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2033</v>
       </c>
       <c r="B16" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH(CpUDSC!A16,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A16,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
         <v>1262597.1562524636</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2034</v>
       </c>
       <c r="B17" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH(CpUDSC!A17,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A17,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
         <v>1247058.3030129359</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2035</v>
       </c>
       <c r="B18" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH(CpUDSC!A18,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A18,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
         <v>1231519.449773408</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2036</v>
       </c>
       <c r="B19" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH(CpUDSC!A19,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A19,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
         <v>1215980.5965338806</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2037</v>
       </c>
       <c r="B20" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH(CpUDSC!A20,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A20,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
         <v>1200441.7432943531</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2038</v>
       </c>
       <c r="B21" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH(CpUDSC!A21,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A21,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
         <v>1184902.8900548255</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2039</v>
       </c>
       <c r="B22" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH(CpUDSC!A22,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A22,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
         <v>1169364.0368152976</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2040</v>
       </c>
       <c r="B23" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH(CpUDSC!A23,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A23,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
         <v>1153825.1835757701</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2041</v>
       </c>
       <c r="B24" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH(CpUDSC!A24,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A24,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
         <v>1138286.3303362424</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2042</v>
       </c>
       <c r="B25" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH(CpUDSC!A25,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A25,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
         <v>1122747.4770967148</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2043</v>
       </c>
       <c r="B26" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH(CpUDSC!A26,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A26,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
         <v>1107208.6238571871</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2044</v>
       </c>
       <c r="B27" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH(CpUDSC!A27,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A27,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
         <v>1091669.7706176594</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2045</v>
       </c>
       <c r="B28" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH(CpUDSC!A28,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A28,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
         <v>1076130.9173781318</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2046</v>
       </c>
       <c r="B29" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH(CpUDSC!A29,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A29,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
         <v>1060592.0641386043</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2047</v>
       </c>
       <c r="B30" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH(CpUDSC!A30,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A30,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
         <v>1045053.2108990765</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2048</v>
       </c>
       <c r="B31" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH(CpUDSC!A31,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A31,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
         <v>1029514.3576595489</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2049</v>
       </c>
       <c r="B32" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH(CpUDSC!A32,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A32,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
         <v>1013975.5044200213</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2050</v>
       </c>
       <c r="B33" s="7">
-        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH(CpUDSC!A33,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
+        <f>(INDEX('NREL ATB'!$C$11:$AI$11,1,MATCH('CpUDSC-totalcost'!A33,'NREL ATB'!$C$3:$AI$3,0))*1000)/'DC to AC'!$A$3</f>
         <v>998436.65118049306</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6139C14F-5B4F-4B7E-AF1C-C0A6186374FC}">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
+  <dimension ref="A1:B33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2019</v>
+      </c>
+      <c r="B2" s="7">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B2</f>
+        <v>1936863.5824986598</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2020</v>
+      </c>
+      <c r="B3" s="7">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B3</f>
+        <v>1831601.6350899425</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2021</v>
+      </c>
+      <c r="B4" s="7">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B4</f>
+        <v>1726339.6876812256</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2022</v>
+      </c>
+      <c r="B5" s="7">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B5</f>
+        <v>1621077.7402725082</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2023</v>
+      </c>
+      <c r="B6" s="7">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B6</f>
+        <v>1515815.7928637911</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2024</v>
+      </c>
+      <c r="B7" s="7">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B7</f>
+        <v>1410553.8454550738</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2025</v>
+      </c>
+      <c r="B8" s="7">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B8</f>
+        <v>1305291.8980463569</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2026</v>
+      </c>
+      <c r="B9" s="7">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B9</f>
+        <v>1200029.9506376397</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2027</v>
+      </c>
+      <c r="B10" s="7">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B10</f>
+        <v>1094768.0032289228</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2028</v>
+      </c>
+      <c r="B11" s="7">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B11</f>
+        <v>989506.05582020571</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2029</v>
+      </c>
+      <c r="B12" s="7">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B12</f>
+        <v>884244.10841148871</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2030</v>
+      </c>
+      <c r="B13" s="7">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B13</f>
+        <v>778982.16100277251</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2031</v>
+      </c>
+      <c r="B14" s="7">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B14</f>
+        <v>769736.54332525376</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2032</v>
+      </c>
+      <c r="B15" s="7">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B15</f>
+        <v>760490.92564773466</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2033</v>
+      </c>
+      <c r="B16" s="7">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B16</f>
+        <v>751245.3079702158</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2034</v>
+      </c>
+      <c r="B17" s="7">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B17</f>
+        <v>741999.69029269682</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2035</v>
+      </c>
+      <c r="B18" s="7">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B18</f>
+        <v>732754.07261517772</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2036</v>
+      </c>
+      <c r="B19" s="7">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B19</f>
+        <v>723508.45493765885</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2037</v>
+      </c>
+      <c r="B20" s="7">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B20</f>
+        <v>714262.83726014011</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2038</v>
+      </c>
+      <c r="B21" s="7">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B21</f>
+        <v>705017.21958262112</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2039</v>
+      </c>
+      <c r="B22" s="7">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B22</f>
+        <v>695771.60190510203</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2040</v>
+      </c>
+      <c r="B23" s="7">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B23</f>
+        <v>686525.98422758316</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2041</v>
+      </c>
+      <c r="B24" s="7">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B24</f>
+        <v>677280.36655006418</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2042</v>
+      </c>
+      <c r="B25" s="7">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B25</f>
+        <v>668034.74887254531</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2043</v>
+      </c>
+      <c r="B26" s="7">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B26</f>
+        <v>658789.13119502633</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2044</v>
+      </c>
+      <c r="B27" s="7">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B27</f>
+        <v>649543.51351750735</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2045</v>
+      </c>
+      <c r="B28" s="7">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B28</f>
+        <v>640297.89583998837</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2046</v>
+      </c>
+      <c r="B29" s="7">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B29</f>
+        <v>631052.27816246951</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2047</v>
+      </c>
+      <c r="B30" s="7">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B30</f>
+        <v>621806.66048495052</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>2048</v>
+      </c>
+      <c r="B31" s="7">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B31</f>
+        <v>612561.04280743154</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>2049</v>
+      </c>
+      <c r="B32" s="7">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B32</f>
+        <v>603315.42512991268</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>2050</v>
+      </c>
+      <c r="B33" s="7">
+        <f>'Soft Cost Data'!$B$10*'CpUDSC-totalcost'!B33</f>
+        <v>594069.80745239335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>